<commit_message>
Rename finalmarkin.py to wr_mark.py. Then changes some names in the file.
</commit_message>
<xml_diff>
--- a/exceltest/电路分析-performance-1621401-2-test.xlsx
+++ b/exceltest/电路分析-performance-1621401-2-test.xlsx
@@ -968,6 +968,9 @@
       <c r="S4" t="n">
         <v>0</v>
       </c>
+      <c r="V4" t="n">
+        <v>88</v>
+      </c>
     </row>
     <row r="5" spans="1:22">
       <c r="B5" t="s">
@@ -1024,6 +1027,9 @@
       <c r="S5" t="n">
         <v>0</v>
       </c>
+      <c r="V5" t="n">
+        <v>88</v>
+      </c>
     </row>
     <row r="6" spans="1:22">
       <c r="B6" t="s">
@@ -1080,6 +1086,9 @@
       <c r="S6" t="n">
         <v>0</v>
       </c>
+      <c r="V6" t="n">
+        <v>79</v>
+      </c>
     </row>
     <row r="7" spans="1:22">
       <c r="B7" t="s">
@@ -1137,7 +1146,7 @@
         <v>0</v>
       </c>
       <c r="V7" t="n">
-        <v>87</v>
+        <v>77</v>
       </c>
     </row>
     <row r="8" spans="1:22">
@@ -1196,7 +1205,7 @@
         <v>0</v>
       </c>
       <c r="V8" t="n">
-        <v>87</v>
+        <v>77</v>
       </c>
     </row>
     <row r="9" spans="1:22">
@@ -1254,6 +1263,9 @@
       <c r="S9" t="n">
         <v>0</v>
       </c>
+      <c r="V9" t="n">
+        <v>77</v>
+      </c>
     </row>
     <row r="10" spans="1:22">
       <c r="B10" t="s">
@@ -1311,7 +1323,7 @@
         <v>0</v>
       </c>
       <c r="V10" t="n">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="11" spans="1:22">
@@ -2840,6 +2852,9 @@
       <c r="S37" t="n">
         <v>0</v>
       </c>
+      <c r="V37" t="n">
+        <v>89</v>
+      </c>
     </row>
     <row r="38" spans="1:22">
       <c r="B38" t="s">
@@ -2897,7 +2912,7 @@
         <v>0</v>
       </c>
       <c r="V38" t="n">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="39" spans="1:22">
@@ -3014,6 +3029,9 @@
       <c r="S40" t="n">
         <v>0</v>
       </c>
+      <c r="V40" t="n">
+        <v>89</v>
+      </c>
     </row>
     <row r="41" spans="1:22">
       <c r="B41" t="s">
@@ -3071,7 +3089,7 @@
         <v>0</v>
       </c>
       <c r="V41" t="n">
-        <v>87</v>
+        <v>92</v>
       </c>
     </row>
     <row r="42" spans="1:22">
@@ -3129,6 +3147,9 @@
       <c r="S42" t="n">
         <v>0</v>
       </c>
+      <c r="V42" t="n">
+        <v>91</v>
+      </c>
     </row>
     <row r="43" spans="1:22">
       <c r="B43" t="s">
@@ -3186,7 +3207,7 @@
         <v>0</v>
       </c>
       <c r="V43" t="n">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="44" spans="1:22">
@@ -3243,6 +3264,9 @@
       </c>
       <c r="S44" t="n">
         <v>0</v>
+      </c>
+      <c r="V44" t="n">
+        <v>91</v>
       </c>
     </row>
     <row r="45" spans="1:22">

</xml_diff>